<commit_message>
@syllabus addition @minor fixes
</commit_message>
<xml_diff>
--- a/edison/assets/xmls/TS_MSB_OnlyReadingsSyllabus.xlsx
+++ b/edison/assets/xmls/TS_MSB_OnlyReadingsSyllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\edison\assets\xmls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thinkSharp\midas\edison\assets\xmls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51DBCCA-4D5E-4B59-941E-A7DEE5D87DFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C322AC86-EDC9-41E9-9292-757711989899}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9017" activeTab="2" xr2:uid="{415AC43A-61C2-4EE4-B405-E644D511166E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{415AC43A-61C2-4EE4-B405-E644D511166E}"/>
   </bookViews>
   <sheets>
     <sheet name="ChapterInfo" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ChapterInfo!$A$1:$G$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1171,22 +1170,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7813A75-25A0-4545-B94D-AE2652D4DB60}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="8.07421875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.61328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.23046875" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.31640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.31640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.58984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.2265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1241,7 +1240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1369,7 +1368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1401,7 +1400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1465,7 +1464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1581,7 +1580,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1607,7 +1606,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1685,7 +1684,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1737,7 +1736,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1945,7 +1944,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1971,7 +1970,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2023,7 +2022,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2101,7 +2100,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2179,7 +2178,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2205,7 +2204,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2361,7 +2360,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2413,7 +2412,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2465,7 +2464,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2517,7 +2516,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2543,7 +2542,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2621,7 +2620,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2699,27 +2698,27 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.75">
       <c r="J57" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.75">
       <c r="J58" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.75">
       <c r="J59" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.75">
       <c r="J60" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.75">
       <c r="J61" t="s">
         <v>145</v>
       </c>
@@ -2737,19 +2736,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875F59B-684D-4223-8F7D-F079E2D97B58}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="18.921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.2265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2792,7 +2791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2832,7 +2831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2872,7 +2871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2952,7 +2951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3012,7 +3011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3052,7 +3051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3072,7 +3071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3092,7 +3091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3132,7 +3131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3192,7 +3191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3212,7 +3211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3252,7 +3251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3292,7 +3291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3332,7 +3331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3372,7 +3371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3392,7 +3391,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3412,7 +3411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3432,7 +3431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3472,7 +3471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3592,7 +3591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3632,7 +3631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3692,7 +3691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3712,7 +3711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3752,7 +3751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3772,7 +3771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3792,7 +3791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3812,7 +3811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3892,7 +3891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3932,7 +3931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3981,17 +3980,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2DAA41-4763-46C2-875C-2EF3C0D615B4}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.2265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4033,7 +4032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4044,7 +4043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4055,7 +4054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4077,7 +4076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4088,7 +4087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4099,7 +4098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4121,7 +4120,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4132,7 +4131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4154,7 +4153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4165,7 +4164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4198,7 +4197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4209,7 +4208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4220,7 +4219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4242,7 +4241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4253,7 +4252,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4264,7 +4263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4286,7 +4285,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4308,7 +4307,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4330,7 +4329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4341,7 +4340,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4352,7 +4351,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4363,7 +4362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4374,7 +4373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4396,7 +4395,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4407,7 +4406,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4429,7 +4428,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4440,7 +4439,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4451,7 +4450,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4462,7 +4461,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4473,7 +4472,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4484,7 +4483,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4506,7 +4505,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4517,7 +4516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4528,7 +4527,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4550,7 +4549,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4561,7 +4560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4572,7 +4571,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4583,7 +4582,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4594,7 +4593,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4605,7 +4604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A56">
         <v>55</v>
       </c>

</xml_diff>